<commit_message>
Add Classes for reamaining pages
</commit_message>
<xml_diff>
--- a/SeleniumPOM/TestData/Guru99Bank.xlsx
+++ b/SeleniumPOM/TestData/Guru99Bank.xlsx
@@ -4,19 +4,31 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="100" windowWidth="19100" windowHeight="7300" activeTab="1"/>
+    <workbookView xWindow="80" yWindow="100" windowWidth="19100" windowHeight="7300" firstSheet="9" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="HomePage" sheetId="1" r:id="rId1"/>
     <sheet name="EditCustomerPage" sheetId="2" r:id="rId2"/>
     <sheet name="NewCustomerPage" sheetId="3" r:id="rId3"/>
+    <sheet name="DeleteCustomer" sheetId="4" r:id="rId4"/>
+    <sheet name="NewAccount" sheetId="5" r:id="rId5"/>
+    <sheet name="EditAccount" sheetId="6" r:id="rId6"/>
+    <sheet name="DeleteAccount" sheetId="7" r:id="rId7"/>
+    <sheet name="Deposit" sheetId="8" r:id="rId8"/>
+    <sheet name="Withdrawal" sheetId="9" r:id="rId9"/>
+    <sheet name="FundTransfer" sheetId="10" r:id="rId10"/>
+    <sheet name="ChangePassword" sheetId="11" r:id="rId11"/>
+    <sheet name="BalanceEnquiry" sheetId="12" r:id="rId12"/>
+    <sheet name="MiniStatement" sheetId="13" r:id="rId13"/>
+    <sheet name="CustomisedStatement" sheetId="14" r:id="rId14"/>
+    <sheet name="Logout" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="19">
   <si>
     <t>Welcome To Manager's Page of Guru99 Bank</t>
   </si>
@@ -472,11 +484,149 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -584,4 +734,146 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="2" max="2" width="17.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="6" customFormat="1" ht="18" customHeight="1">
+      <c r="A1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="4" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added testcases for remaining pages
</commit_message>
<xml_diff>
--- a/SeleniumPOM/TestData/Guru99Bank.xlsx
+++ b/SeleniumPOM/TestData/Guru99Bank.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="100" windowWidth="19100" windowHeight="7300" firstSheet="9" activeTab="14"/>
+    <workbookView xWindow="80" yWindow="100" windowWidth="19100" windowHeight="7300" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="HomePage" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="19">
   <si>
     <t>Welcome To Manager's Page of Guru99 Bank</t>
   </si>
@@ -486,6 +486,201 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -507,127 +702,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:2" s="4" customFormat="1">
-      <c r="A1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:2" s="4" customFormat="1">
-      <c r="A1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:2" s="4" customFormat="1">
-      <c r="A1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:2" s="4" customFormat="1">
-      <c r="A1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:2" s="4" customFormat="1">
-      <c r="A1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -738,10 +818,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -757,6 +837,22 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -765,20 +861,36 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:2" s="4" customFormat="1">
-      <c r="A1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>5</v>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -788,10 +900,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -804,6 +916,22 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -811,20 +939,36 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:2" s="4" customFormat="1">
-      <c r="A1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>5</v>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -834,20 +978,36 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:2" s="4" customFormat="1">
-      <c r="A1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>5</v>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -857,20 +1017,36 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:2" s="4" customFormat="1">
-      <c r="A1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>5</v>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added TestReports and Mail API
</commit_message>
<xml_diff>
--- a/SeleniumPOM/TestData/Guru99Bank.xlsx
+++ b/SeleniumPOM/TestData/Guru99Bank.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="100" windowWidth="19100" windowHeight="7300"/>
+    <workbookView xWindow="80" yWindow="100" windowWidth="19100" windowHeight="7300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="HomePage" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="16">
   <si>
     <t>Welcome To Manager's Page of Guru99 Bank</t>
   </si>
@@ -60,21 +60,9 @@
     <t>Special characters are not allowed</t>
   </si>
   <si>
-    <t xml:space="preserve">          </t>
-  </si>
-  <si>
     <t>abcdefghijklmnopqrstuvwxyz</t>
   </si>
   <si>
-    <t>Numbers are not allowed</t>
-  </si>
-  <si>
-    <t>Special characters are not allowed</t>
-  </si>
-  <si>
-    <t>First character can not have space</t>
-  </si>
-  <si>
     <t>MaxCharacter</t>
   </si>
   <si>
@@ -84,14 +72,17 @@
     <t>BlankMessage</t>
   </si>
   <si>
-    <t>Customer name must not be blank</t>
+    <t>Customer name must not be blank</t>
+  </si>
+  <si>
+    <t>Numbers are not allowed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +102,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -139,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -157,6 +154,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,7 +451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -746,17 +744,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="29.54296875" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.36328125" customWidth="1"/>
-    <col min="5" max="5" width="28.81640625" customWidth="1"/>
+    <col min="5" max="5" width="33.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="13.5" customHeight="1">
@@ -767,50 +765,35 @@
         <v>5</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16" customHeight="1">
       <c r="A2">
         <v>123456</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>12</v>
+      <c r="B2" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>25</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="E2" s="9" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>